<commit_message>
Updated with 2025 data and updated data template
</commit_message>
<xml_diff>
--- a/data/spawner_count_template.xlsx
+++ b/data/spawner_count_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://freshwaterfisheries-my.sharepoint.com/personal/paul_askey_gofishbc_com/Documents/FFSBC work docs/Git_projects/KokaneeSpawnerApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{09919641-852E-4D86-B152-1BB89FC55193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCE09EFB-1BAE-4D93-A025-1C04670CDF6E}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="8_{09919641-852E-4D86-B152-1BB89FC55193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B13F465-243D-4F01-8C35-96510108A0A0}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1161,7 +1161,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11214,7 +11214,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
+  <dataValidations count="13">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"OKANAGAN,KALAMALKA,WOOD,SKAHA"</formula1>
     </dataValidation>
@@ -11226,7 +11226,7 @@
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" error="Day must be between 1 and 31." sqref="I2:J1000" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" error="Day must be between 1 and 31." sqref="I2:I1000" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>1</formula1>
       <formula2>31</formula2>
     </dataValidation>
@@ -11255,6 +11255,10 @@
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{8257D202-68A8-454A-A7B1-112F791105D3}">
       <formula1>"STREAM, SHORE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" error="Time entered as integer number with no semi-colon" sqref="J2:J1000" xr:uid="{51E98EDB-40B5-4852-A436-148455142BB6}">
+      <formula1>700</formula1>
+      <formula2>2000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>